<commit_message>
Update Tesis indicador de versiones.xlsx
</commit_message>
<xml_diff>
--- a/Ante Proyecto/Tesis indicador de versiones.xlsx
+++ b/Ante Proyecto/Tesis indicador de versiones.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>TABLA DE ORGANIZACIÓN DE INFORMACION DE TESIS</t>
   </si>
@@ -175,13 +175,19 @@
   </si>
   <si>
     <t>resistencia al impacto en plásticossegun metodo Izod</t>
+  </si>
+  <si>
+    <t>Version 3</t>
+  </si>
+  <si>
+    <t>Evaluación de la Biocompatibilidad y el Rendimiento Mecánico de Alineadores Ortodónticos Monocapa (PET-G) y Tricapa (PU-Copolímero) en Contacto con Tejidos Orales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +226,13 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -267,10 +280,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -282,19 +307,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -630,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N37"/>
+  <dimension ref="B2:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -645,587 +664,737 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
     <row r="3" spans="2:14">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" spans="2:14">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
     </row>
     <row r="5" spans="2:14">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
     </row>
     <row r="6" spans="2:14">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
     </row>
     <row r="8" spans="2:14">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="5" t="s">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
     </row>
     <row r="10" spans="2:14">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
     </row>
     <row r="11" spans="2:14">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
     </row>
     <row r="12" spans="2:14">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
     </row>
     <row r="13" spans="2:14">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
     </row>
     <row r="14" spans="2:14">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
     </row>
     <row r="15" spans="2:14">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
     </row>
     <row r="16" spans="2:14">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
     </row>
     <row r="17" spans="2:14">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
     </row>
     <row r="18" spans="2:14">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
     </row>
     <row r="19" spans="2:14">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
     </row>
     <row r="20" spans="2:14" ht="27.75">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
     </row>
     <row r="21" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2" t="s">
+      <c r="E21" s="6"/>
+      <c r="F21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="5" t="s">
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
     </row>
     <row r="22" spans="2:14">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
     </row>
     <row r="23" spans="2:14">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
     </row>
     <row r="24" spans="2:14">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
     </row>
     <row r="25" spans="2:14">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="1" t="s">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
     </row>
     <row r="26" spans="2:14">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
     </row>
     <row r="27" spans="2:14">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
     </row>
     <row r="28" spans="2:14">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
     </row>
     <row r="29" spans="2:14">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="1" t="s">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
     </row>
     <row r="30" spans="2:14">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
     </row>
     <row r="31" spans="2:14">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
     </row>
     <row r="32" spans="2:14">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
     </row>
     <row r="33" spans="2:14">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="1" t="s">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
     </row>
     <row r="34" spans="2:14">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
     </row>
     <row r="35" spans="2:14">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
     </row>
     <row r="36" spans="2:14">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
     </row>
     <row r="37" spans="2:14" ht="26.25">
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+    </row>
+    <row r="39" spans="2:14" ht="14.25" customHeight="1">
+      <c r="B39" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="11"/>
+      <c r="D39" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" spans="2:14">
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+    </row>
+    <row r="41" spans="2:14">
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" spans="2:14">
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+    </row>
+    <row r="43" spans="2:14">
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+    </row>
+    <row r="44" spans="2:14">
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+    </row>
+    <row r="45" spans="2:14">
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+    </row>
+    <row r="46" spans="2:14">
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+    </row>
+    <row r="47" spans="2:14">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+    </row>
+    <row r="48" spans="2:14">
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+    </row>
+    <row r="53" spans="2:8">
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="23">
+    <mergeCell ref="B39:C53"/>
+    <mergeCell ref="D39:E53"/>
+    <mergeCell ref="F39:H53"/>
+    <mergeCell ref="I33:N36"/>
+    <mergeCell ref="B21:C36"/>
+    <mergeCell ref="D21:E36"/>
+    <mergeCell ref="F21:H36"/>
+    <mergeCell ref="B37:N37"/>
+    <mergeCell ref="I21:N24"/>
+    <mergeCell ref="I25:N28"/>
+    <mergeCell ref="I29:N32"/>
     <mergeCell ref="B2:N4"/>
     <mergeCell ref="I8:N11"/>
     <mergeCell ref="I12:N15"/>
@@ -1238,14 +1407,6 @@
     <mergeCell ref="B8:C19"/>
     <mergeCell ref="D8:E19"/>
     <mergeCell ref="F8:H19"/>
-    <mergeCell ref="I33:N36"/>
-    <mergeCell ref="B21:C36"/>
-    <mergeCell ref="D21:E36"/>
-    <mergeCell ref="F21:H36"/>
-    <mergeCell ref="B37:N37"/>
-    <mergeCell ref="I21:N24"/>
-    <mergeCell ref="I25:N28"/>
-    <mergeCell ref="I29:N32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1267,62 +1428,62 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6" t="s">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="6"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="2:11">
       <c r="B7" s="9" t="s">
@@ -1334,11 +1495,11 @@
         <v>31</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
     </row>
@@ -1348,9 +1509,9 @@
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
@@ -1360,9 +1521,9 @@
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
     </row>
@@ -1372,9 +1533,9 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
     </row>
@@ -1384,9 +1545,9 @@
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
     </row>
@@ -1400,11 +1561,11 @@
         <v>32</v>
       </c>
       <c r="F12" s="9"/>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
     </row>
@@ -1414,9 +1575,9 @@
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
     </row>
@@ -1426,9 +1587,9 @@
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
     </row>
@@ -1438,9 +1599,9 @@
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
     </row>
@@ -1450,9 +1611,9 @@
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
     </row>
@@ -1466,11 +1627,11 @@
         <v>33</v>
       </c>
       <c r="F17" s="9"/>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
     </row>
@@ -1480,9 +1641,9 @@
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
     </row>
@@ -1492,9 +1653,9 @@
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
     </row>
@@ -1504,9 +1665,9 @@
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
     </row>
@@ -1516,9 +1677,9 @@
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
     </row>
@@ -1598,11 +1759,11 @@
         <v>35</v>
       </c>
       <c r="F27" s="9"/>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
     </row>
@@ -1612,9 +1773,9 @@
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
     </row>
@@ -1624,9 +1785,9 @@
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
     </row>
@@ -1636,9 +1797,9 @@
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
     </row>
@@ -1648,9 +1809,9 @@
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
     </row>
@@ -1664,11 +1825,11 @@
         <v>43</v>
       </c>
       <c r="F32" s="9"/>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
     </row>
@@ -1678,9 +1839,9 @@
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
     </row>
@@ -1690,9 +1851,9 @@
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
     </row>
@@ -1702,9 +1863,9 @@
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
     </row>
@@ -1714,27 +1875,14 @@
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B7:D11"/>
-    <mergeCell ref="E7:F11"/>
-    <mergeCell ref="B17:D21"/>
-    <mergeCell ref="E17:F21"/>
-    <mergeCell ref="G17:I21"/>
-    <mergeCell ref="B22:D26"/>
-    <mergeCell ref="E22:F26"/>
-    <mergeCell ref="G22:I26"/>
-    <mergeCell ref="B3:K4"/>
-    <mergeCell ref="B5:D6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="G5:I6"/>
-    <mergeCell ref="J5:K6"/>
     <mergeCell ref="B32:D36"/>
     <mergeCell ref="E32:F36"/>
     <mergeCell ref="G32:I36"/>
@@ -1751,6 +1899,19 @@
     <mergeCell ref="J17:K21"/>
     <mergeCell ref="J22:K26"/>
     <mergeCell ref="J27:K31"/>
+    <mergeCell ref="B22:D26"/>
+    <mergeCell ref="E22:F26"/>
+    <mergeCell ref="G22:I26"/>
+    <mergeCell ref="B3:K4"/>
+    <mergeCell ref="B5:D6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="G5:I6"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="B7:D11"/>
+    <mergeCell ref="E7:F11"/>
+    <mergeCell ref="B17:D21"/>
+    <mergeCell ref="E17:F21"/>
+    <mergeCell ref="G17:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>